<commit_message>
Added Marks to added features
</commit_message>
<xml_diff>
--- a/Management/PRODUCTION/PRIORITIES.xlsx
+++ b/Management/PRODUCTION/PRIORITIES.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\GDC2017Project\Management\PRODUCTION\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="19560" windowHeight="8010"/>
   </bookViews>
@@ -183,8 +188,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,13 +209,35 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C5700"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -222,10 +249,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,8 +265,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -245,6 +288,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -293,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,9 +372,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,6 +424,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,13 +620,13 @@
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.796875" style="1"/>
-    <col min="3" max="3" width="9.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
@@ -556,34 +636,34 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -641,34 +721,34 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+      <c r="B15" s="6">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>13</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+      <c r="B17" s="6">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>